<commit_message>
updated recalculation of Excel files.
</commit_message>
<xml_diff>
--- a/data/eta_i.xlsx
+++ b/data/eta_i.xlsx
@@ -1,137 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E5ABBE-450F-D64D-9AB0-B910687B6CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19020" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" windowHeight="13125" windowWidth="13125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>machine</t>
-  </si>
-  <si>
-    <t>eta_i</t>
-  </si>
-  <si>
-    <t>Blast furnace</t>
-  </si>
-  <si>
-    <t>Blast furnaces</t>
-  </si>
-  <si>
-    <t>Charcoal production plants</t>
-  </si>
-  <si>
-    <t>CO gas treatment</t>
-  </si>
-  <si>
-    <t>Coal beneficiation</t>
-  </si>
-  <si>
-    <t>Coal extraction</t>
-  </si>
-  <si>
-    <t>Coal hauling</t>
-  </si>
-  <si>
-    <t>Coal liquefaction plants</t>
-  </si>
-  <si>
-    <t>Coal mines</t>
-  </si>
-  <si>
-    <t>Coke oven</t>
-  </si>
-  <si>
-    <t>Coke ovens</t>
-  </si>
-  <si>
-    <t>Gas works</t>
-  </si>
-  <si>
-    <t>Gas-to-liquids (GTL) plants</t>
-  </si>
-  <si>
-    <t>Iron ore beneficiation</t>
-  </si>
-  <si>
-    <t>Iron ore extraction</t>
-  </si>
-  <si>
-    <t>Iron ore hauling</t>
-  </si>
-  <si>
-    <t>Limestone beneficiation</t>
-  </si>
-  <si>
-    <t>Limestone extraction</t>
-  </si>
-  <si>
-    <t>Limestone hauling</t>
-  </si>
-  <si>
-    <t>Main activity producer electricity plants</t>
-  </si>
-  <si>
-    <t>Manufacture [of Hydro]</t>
-  </si>
-  <si>
-    <t>Manufacture [of Nuclear]</t>
-  </si>
-  <si>
-    <t>Manufacture [of Primary solid biofuels]</t>
-  </si>
-  <si>
-    <t>Manufacture [of Solar photovoltaics]</t>
-  </si>
-  <si>
-    <t>Manufacture [of Solar thermal]</t>
-  </si>
-  <si>
-    <t>Manufacture [of Wind]</t>
-  </si>
-  <si>
-    <t>Mixer</t>
-  </si>
-  <si>
-    <t>Natural gas extraction</t>
-  </si>
-  <si>
-    <t>Nuclear industry</t>
-  </si>
-  <si>
-    <t>Oil extraction</t>
-  </si>
-  <si>
-    <t>Oil refineries</t>
-  </si>
-  <si>
-    <t>Rotary kiln</t>
-  </si>
-  <si>
-    <t>Transfers</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,15 +49,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -495,292 +368,357 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>machine</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>eta_i</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Blast furnace</t>
+        </is>
       </c>
       <c r="B2">
-        <v>0.33030596672893298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
+        <v>0.330305966728933</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Blast furnaces</t>
+        </is>
       </c>
       <c r="B3">
         <v>0.396190004315019</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Charcoal production plants</t>
+        </is>
       </c>
       <c r="B4">
         <v>0.144782108619289</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CO gas treatment</t>
+        </is>
       </c>
       <c r="B5">
         <v>0.993158562772116</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Coal beneficiation</t>
+        </is>
       </c>
       <c r="B6">
         <v>0.9967429853184</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Coal extraction</t>
+        </is>
       </c>
       <c r="B7">
-        <v>0.98878157674342804</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
+        <v>0.988781576743428</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Coal hauling</t>
+        </is>
       </c>
       <c r="B8">
-        <v>0.98202222166069097</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
+        <v>0.982022221660691</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Coal liquefaction plants</t>
+        </is>
       </c>
       <c r="B9">
-        <v>0.20009337306959599</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
+        <v>0.200093373069596</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Coal mines</t>
+        </is>
       </c>
       <c r="B10">
-        <v>0.99818545824480898</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
+        <v>0.998185458244809</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Coke oven</t>
+        </is>
       </c>
       <c r="B11">
         <v>1.21401421645458</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Coke ovens</t>
+        </is>
       </c>
       <c r="B12">
         <v>0.69162956344699</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Gas works</t>
+        </is>
       </c>
       <c r="B13">
-        <v>0.26391004835057602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
+        <v>0.263910048350576</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Gas-to-liquids (GTL) plants</t>
+        </is>
       </c>
       <c r="B14">
-        <v>0.54320718242047505</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
+        <v>0.543207182420475</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Iron ore beneficiation</t>
+        </is>
       </c>
       <c r="B15">
-        <v>0.90849653604279901</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
+        <v>0.908496536042799</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Iron ore extraction</t>
+        </is>
       </c>
       <c r="B16">
         <v>0.548347890347756</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>17</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Iron ore hauling</t>
+        </is>
       </c>
       <c r="B17">
-        <v>0.15191900995389199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>18</v>
+        <v>0.151919009953892</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Limestone beneficiation</t>
+        </is>
       </c>
       <c r="B18">
         <v>0.99863627332533</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>19</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Limestone extraction</t>
+        </is>
       </c>
       <c r="B19">
         <v>0.989269084550077</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>20</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Limestone hauling</t>
+        </is>
       </c>
       <c r="B20">
-        <v>0.89989464623142001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
+        <v>0.89989464623142</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Main activity producer electricity plants</t>
+        </is>
       </c>
       <c r="B21">
-        <v>0.31451970596399298</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>22</v>
+        <v>0.314519705963993</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Manufacture [of Hydro]</t>
+        </is>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>23</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Manufacture [of Nuclear]</t>
+        </is>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Manufacture [of Primary solid biofuels]</t>
+        </is>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>25</v>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Manufacture [of Solar photovoltaics]</t>
+        </is>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>26</v>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Manufacture [of Solar thermal]</t>
+        </is>
       </c>
       <c r="B26" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>27</v>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Manufacture [of Wind]</t>
+        </is>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>28</v>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Mixer</t>
+        </is>
       </c>
       <c r="B28">
-        <v>0.99300939590335402</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>29</v>
+        <v>0.993009395903354</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Natural gas extraction</t>
+        </is>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>30</v>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Nuclear industry</t>
+        </is>
       </c>
       <c r="B30">
-        <v>0.33000000000000501</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>31</v>
+        <v>0.330000000000005</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Oil extraction</t>
+        </is>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>32</v>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Oil refineries</t>
+        </is>
       </c>
       <c r="B32">
-        <v>0.92196039018737497</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>33</v>
+        <v>0.921960390187375</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Rotary kiln</t>
+        </is>
       </c>
       <c r="B33">
-        <v>1.0532312287483201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>34</v>
+        <v>1.05323122874832</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Transfers</t>
+        </is>
       </c>
       <c r="B34">
-        <v>1.0703178798177599</v>
+        <v>1.07031787981776</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="1"/>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to all data files.
</commit_message>
<xml_diff>
--- a/data/eta_i.xlsx
+++ b/data/eta_i.xlsx
@@ -394,7 +394,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.379430224241158</v>
+        <v>0.379390578971147</v>
       </c>
     </row>
     <row r="3">
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.991749634631216</v>
+        <v>0.99193886757516</v>
       </c>
     </row>
     <row r="25">

</xml_diff>